<commit_message>
Add total individuals to output
</commit_message>
<xml_diff>
--- a/ons-income-2022/hdi_composition_nonretired.xlsx
+++ b/ons-income-2022/hdi_composition_nonretired.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mr_cp\git\household_expenses_analysis\ons-income-2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E435C5-5370-4F3E-AF4A-64E7A97E6401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1930EB25-E625-40D8-BFB1-08E4D8BDA1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{85EDC0DB-47F5-46C4-9D0E-6BDBB92946E1}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11160" activeTab="5" xr2:uid="{85EDC0DB-47F5-46C4-9D0E-6BDBB92946E1}"/>
   </bookViews>
   <sheets>
     <sheet name="composition" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,10 @@
     <sheet name="deciles_edges" sheetId="12" r:id="rId3"/>
     <sheet name="deciles" sheetId="2" r:id="rId4"/>
     <sheet name="n_households" sheetId="10" r:id="rId5"/>
-    <sheet name="income" sheetId="8" r:id="rId6"/>
-    <sheet name="benefits" sheetId="9" r:id="rId7"/>
-    <sheet name="taxes" sheetId="7" r:id="rId8"/>
+    <sheet name="n_individuals" sheetId="13" r:id="rId6"/>
+    <sheet name="income" sheetId="8" r:id="rId7"/>
+    <sheet name="benefits" sheetId="9" r:id="rId8"/>
+    <sheet name="taxes" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
   <si>
     <t>Non-retired</t>
   </si>
@@ -178,6 +179,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 3 or more adults with children</t>
+  </si>
+  <si>
+    <t>Number of individuals in the population ('000s)</t>
   </si>
 </sst>
 </file>
@@ -661,7 +665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82AC85D4-D29F-4C53-95D9-752174396079}">
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="M2" sqref="M2:M9"/>
     </sheetView>
   </sheetViews>
@@ -21676,6 +21680,31 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F03D3370-C09C-4F46-BE5F-9AC82BEC0BF9}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="21">
+        <v>54742</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB9F16C-B8FB-45BB-A185-5BEC4EF9E56F}">
   <dimension ref="A1:M351"/>
   <sheetViews>
@@ -26970,7 +26999,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E8294A-8B0F-4099-942B-F6C21328647A}">
   <dimension ref="A1:M367"/>
   <sheetViews>
@@ -32889,7 +32918,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{516A9811-EB4C-4FCB-BDB5-1E3C501726F7}">
   <dimension ref="A1:M349"/>
   <sheetViews>

</xml_diff>